<commit_message>
added tsv parsing and adding to db
</commit_message>
<xml_diff>
--- a/docs/integratsiiapparatnyhpl.xlsx
+++ b/docs/integratsiiapparatnyhpl.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tankovds\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iljad\Desktop\Pets\Go\BIOCAD\test task\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0B0A36DB-2F07-43F4-B7B3-C809062E995A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF186746-C450-4000-A9E2-DF48A9960839}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B1FA5221-B8ED-4C76-9596-6C5AFC5DFD42}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B1FA5221-B8ED-4C76-9596-6C5AFC5DFD42}"/>
   </bookViews>
   <sheets>
     <sheet name="Задание" sheetId="1" r:id="rId1"/>
@@ -24,12 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -341,7 +336,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -397,9 +392,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -437,7 +432,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -543,7 +538,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -699,9 +694,9 @@
       <selection activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -725,7 +720,7 @@
       <c r="S1" s="2"/>
       <c r="T1" s="2"/>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -747,7 +742,7 @@
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -769,7 +764,7 @@
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -791,7 +786,7 @@
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -813,7 +808,7 @@
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -835,7 +830,7 @@
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -857,7 +852,7 @@
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -879,7 +874,7 @@
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -901,7 +896,7 @@
       <c r="S9" s="2"/>
       <c r="T9" s="2"/>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -923,7 +918,7 @@
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -945,7 +940,7 @@
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -967,7 +962,7 @@
       <c r="S12" s="2"/>
       <c r="T12" s="2"/>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -989,7 +984,7 @@
       <c r="S13" s="2"/>
       <c r="T13" s="2"/>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1011,7 +1006,7 @@
       <c r="S14" s="2"/>
       <c r="T14" s="2"/>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -1033,7 +1028,7 @@
       <c r="S15" s="2"/>
       <c r="T15" s="2"/>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1055,7 +1050,7 @@
       <c r="S16" s="2"/>
       <c r="T16" s="2"/>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -1077,7 +1072,7 @@
       <c r="S17" s="2"/>
       <c r="T17" s="2"/>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -1099,7 +1094,7 @@
       <c r="S18" s="2"/>
       <c r="T18" s="2"/>
     </row>
-    <row r="19" spans="1:20">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1121,7 +1116,7 @@
       <c r="S19" s="2"/>
       <c r="T19" s="2"/>
     </row>
-    <row r="20" spans="1:20">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1143,7 +1138,7 @@
       <c r="S20" s="2"/>
       <c r="T20" s="2"/>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -1165,7 +1160,7 @@
       <c r="S21" s="2"/>
       <c r="T21" s="2"/>
     </row>
-    <row r="22" spans="1:20">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1187,7 +1182,7 @@
       <c r="S22" s="2"/>
       <c r="T22" s="2"/>
     </row>
-    <row r="23" spans="1:20">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -1209,7 +1204,7 @@
       <c r="S23" s="2"/>
       <c r="T23" s="2"/>
     </row>
-    <row r="24" spans="1:20">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1231,7 +1226,7 @@
       <c r="S24" s="2"/>
       <c r="T24" s="2"/>
     </row>
-    <row r="25" spans="1:20">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1253,7 +1248,7 @@
       <c r="S25" s="2"/>
       <c r="T25" s="2"/>
     </row>
-    <row r="26" spans="1:20">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -1275,7 +1270,7 @@
       <c r="S26" s="2"/>
       <c r="T26" s="2"/>
     </row>
-    <row r="27" spans="1:20">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -1297,7 +1292,7 @@
       <c r="S27" s="2"/>
       <c r="T27" s="2"/>
     </row>
-    <row r="28" spans="1:20">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -1319,7 +1314,7 @@
       <c r="S28" s="2"/>
       <c r="T28" s="2"/>
     </row>
-    <row r="29" spans="1:20">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1341,7 +1336,7 @@
       <c r="S29" s="2"/>
       <c r="T29" s="2"/>
     </row>
-    <row r="30" spans="1:20">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -1363,7 +1358,7 @@
       <c r="S30" s="2"/>
       <c r="T30" s="2"/>
     </row>
-    <row r="31" spans="1:20">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -1385,7 +1380,7 @@
       <c r="S31" s="2"/>
       <c r="T31" s="2"/>
     </row>
-    <row r="32" spans="1:20">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -1407,7 +1402,7 @@
       <c r="S32" s="2"/>
       <c r="T32" s="2"/>
     </row>
-    <row r="33" spans="1:20">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -1429,7 +1424,7 @@
       <c r="S33" s="2"/>
       <c r="T33" s="2"/>
     </row>
-    <row r="34" spans="1:20">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -1465,12 +1460,12 @@
   <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1514,7 +1509,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1561,7 +1556,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -1596,7 +1591,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -1631,7 +1626,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -1666,7 +1661,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -1701,7 +1696,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>54</v>
       </c>
@@ -1736,7 +1731,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>59</v>
       </c>
@@ -1771,7 +1766,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>62</v>
       </c>
@@ -1806,7 +1801,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>65</v>
       </c>
@@ -1841,7 +1836,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>68</v>
       </c>
@@ -1876,7 +1871,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1911,7 +1906,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1946,7 +1941,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1981,7 +1976,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2016,7 +2011,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2051,7 +2046,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2086,7 +2081,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -2121,7 +2116,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>16</v>
       </c>
@@ -2156,7 +2151,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>16</v>
       </c>
@@ -2209,15 +2204,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Документ" ma:contentTypeID="0x01010032881369D53B13439A3FE46DCBBFF391" ma:contentTypeVersion="16" ma:contentTypeDescription="Создание документа." ma:contentTypeScope="" ma:versionID="1a4c69d6f4be7df474a7892c5239afe6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2c3df61b-3502-4f10-a533-735981e934da" xmlns:ns3="9a87fd55-1da1-4d46-a5a8-4ddc854d8cb1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="016cfad7b387a66efc12e70fa9836e94" ns2:_="" ns3:_="">
     <xsd:import namespace="2c3df61b-3502-4f10-a533-735981e934da"/>
@@ -2460,14 +2446,49 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54734E02-F74C-4B49-93F6-1B01949943E8}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54734E02-F74C-4B49-93F6-1B01949943E8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2c3df61b-3502-4f10-a533-735981e934da"/>
+    <ds:schemaRef ds:uri="9a87fd55-1da1-4d46-a5a8-4ddc854d8cb1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65CB87D0-74ED-4EE0-A640-505294E264D3}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D49F1B1-40AB-42A7-B581-6FFBCD3E8E92}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2c3df61b-3502-4f10-a533-735981e934da"/>
+    <ds:schemaRef ds:uri="9a87fd55-1da1-4d46-a5a8-4ddc854d8cb1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D49F1B1-40AB-42A7-B581-6FFBCD3E8E92}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65CB87D0-74ED-4EE0-A640-505294E264D3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>